<commit_message>
Summary box vs title box resolved
</commit_message>
<xml_diff>
--- a/Books_Info.xlsx
+++ b/Books_Info.xlsx
@@ -28,13 +28,13 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>Automata and omputability</t>
-  </si>
-  <si>
-    <t>['KozEN']</t>
-  </si>
-  <si>
-    <t>['Springer']</t>
+    <t>THE POWER OF YOU</t>
+  </si>
+  <si>
+    <t>['Somsbodvfamou ruccetful', 'Timg', 'Thi', 'blackbelt', 'Oere Mucy Cenb', 'THE POWER OF YOU']</t>
+  </si>
+  <si>
+    <t>['Forbes', 'U.N']</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
filetypes and directorued handled
</commit_message>
<xml_diff>
--- a/Books_Info.xlsx
+++ b/Books_Info.xlsx
@@ -28,13 +28,13 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>THE POWER OF YOU</t>
-  </si>
-  <si>
-    <t>['Somsbodvfamou ruccetful', 'Timg', 'Thi', 'blackbelt', 'Oere Mucy Cenb', 'THE POWER OF YOU']</t>
-  </si>
-  <si>
-    <t>['Forbes', 'U.N']</t>
+    <t>Clean Code A Handbook of Agile Software Craftsmanship</t>
+  </si>
+  <si>
+    <t>['James 0. Coplien', 'Robert C Martin']</t>
+  </si>
+  <si>
+    <t>['PReNtICE HALL']</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fixed bugs, todo - barcode, json, all string publisher, make author and publisher list a set
</commit_message>
<xml_diff>
--- a/Books_Info.xlsx
+++ b/Books_Info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Title</t>
   </si>
@@ -28,13 +28,19 @@
     <t>Publisher</t>
   </si>
   <si>
+    <t>MY BOOK  COVER Secrets in a Silicon Valley Startup</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
     <t>Clean Code A Handbook of Agile Software Craftsmanship</t>
   </si>
   <si>
     <t>['James 0. Coplien', 'Robert C Martin']</t>
   </si>
   <si>
-    <t>['PReNtICE HALL']</t>
+    <t>['Prentice Hall Ptr']</t>
   </si>
 </sst>
 </file>
@@ -366,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -394,7 +400,18 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added barcode isbn, all strings publisher, tests tbd
</commit_message>
<xml_diff>
--- a/Books_Info.xlsx
+++ b/Books_Info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Title</t>
   </si>
@@ -28,19 +28,16 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>MY BOOK  COVER Secrets in a Silicon Valley Startup</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>Clean Code A Handbook of Agile Software Craftsmanship</t>
-  </si>
-  <si>
-    <t>['James 0. Coplien', 'Robert C Martin']</t>
-  </si>
-  <si>
-    <t>['Prentice Hall Ptr']</t>
+    <t>Agile Methodology Master the art of Software Development:</t>
+  </si>
+  <si>
+    <t>978-0-618-26030-0</t>
+  </si>
+  <si>
+    <t>['Jason Roy', 'John Jacob Henry Rose']</t>
+  </si>
+  <si>
+    <t>['The MIT Press']</t>
   </si>
 </sst>
 </file>
@@ -372,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,22 +393,14 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>